<commit_message>
update import mockData and monthly used KwH stored per month
</commit_message>
<xml_diff>
--- a/src/mockData.xlsx
+++ b/src/mockData.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\educom-ecopowrrr\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF32DF41-038C-470A-980A-8014C5AFC8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990DB15A-0D81-4000-A3C3-E3DA23019C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{D355C713-1B71-42EE-97C5-B7799D081BF6}"/>
+    <workbookView xWindow="-28905" yWindow="-8025" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{D355C713-1B71-42EE-97C5-B7799D081BF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Client" sheetId="1" r:id="rId1"/>
-    <sheet name="Device" sheetId="2" r:id="rId2"/>
-    <sheet name="Price" sheetId="5" r:id="rId3"/>
-    <sheet name="DeviceMetrics" sheetId="3" r:id="rId4"/>
+    <sheet name="MonthlyUsed" sheetId="7" r:id="rId2"/>
+    <sheet name="Device" sheetId="2" r:id="rId3"/>
+    <sheet name="Price" sheetId="5" r:id="rId4"/>
+    <sheet name="DeviceMetrics" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="124">
   <si>
     <t>id</t>
   </si>
@@ -51,6 +52,9 @@
   </si>
   <si>
     <t>endDate</t>
+  </si>
+  <si>
+    <t>monthlyKwHUsed</t>
   </si>
   <si>
     <t>deviceId</t>
@@ -793,7 +797,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B6" sqref="B6:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -803,31 +807,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -835,31 +839,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E2">
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -867,31 +871,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H3">
         <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -899,31 +903,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4">
         <v>59</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -931,31 +935,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E5">
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H5">
         <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -966,28 +970,28 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H6">
         <v>61</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -998,28 +1002,28 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E7">
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H7">
         <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1030,28 +1034,28 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E8">
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H8">
         <v>40</v>
       </c>
       <c r="I8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1062,28 +1066,28 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H9">
         <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1094,28 +1098,28 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H10">
         <v>81</v>
       </c>
       <c r="I10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1126,28 +1130,28 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H11">
         <v>23</v>
       </c>
       <c r="I11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1158,28 +1162,28 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E12">
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H12">
         <v>45</v>
       </c>
       <c r="I12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1190,28 +1194,28 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H13">
         <v>67</v>
       </c>
       <c r="I13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1222,28 +1226,28 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14">
         <v>55</v>
       </c>
       <c r="F14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H14">
         <v>54</v>
       </c>
       <c r="I14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1252,10 +1256,1554 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA159A3-303D-40FE-977A-C1EB7FDBEF5E}">
+  <dimension ref="A1:D109"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45322</v>
+      </c>
+      <c r="D2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45351</v>
+      </c>
+      <c r="D3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45382</v>
+      </c>
+      <c r="D4">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>45412</v>
+      </c>
+      <c r="D5">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>45443</v>
+      </c>
+      <c r="D6">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45473</v>
+      </c>
+      <c r="D7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D8">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>45535</v>
+      </c>
+      <c r="D9">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>45565</v>
+      </c>
+      <c r="D10">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D11">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D12">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D13">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>45322</v>
+      </c>
+      <c r="D14">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>45351</v>
+      </c>
+      <c r="D15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>45382</v>
+      </c>
+      <c r="D16">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2">
+        <v>45412</v>
+      </c>
+      <c r="D17">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>45443</v>
+      </c>
+      <c r="D18">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2">
+        <v>45473</v>
+      </c>
+      <c r="D19">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D20">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2">
+        <v>45535</v>
+      </c>
+      <c r="D21">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>45565</v>
+      </c>
+      <c r="D22">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D23">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D24">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>45322</v>
+      </c>
+      <c r="D26">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2">
+        <v>45351</v>
+      </c>
+      <c r="D27">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2">
+        <v>45382</v>
+      </c>
+      <c r="D28">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" s="2">
+        <v>45412</v>
+      </c>
+      <c r="D29">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2">
+        <v>45443</v>
+      </c>
+      <c r="D30">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" s="2">
+        <v>45473</v>
+      </c>
+      <c r="D31">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D32">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" s="2">
+        <v>45535</v>
+      </c>
+      <c r="D33">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" s="2">
+        <v>45565</v>
+      </c>
+      <c r="D34">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D36">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D37">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2">
+        <v>45322</v>
+      </c>
+      <c r="D38">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" s="2">
+        <v>45351</v>
+      </c>
+      <c r="D39">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" s="2">
+        <v>45382</v>
+      </c>
+      <c r="D40">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" s="2">
+        <v>45412</v>
+      </c>
+      <c r="D41">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42" s="2">
+        <v>45443</v>
+      </c>
+      <c r="D42">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43" s="2">
+        <v>45473</v>
+      </c>
+      <c r="D43">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D44">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45" s="2">
+        <v>45535</v>
+      </c>
+      <c r="D45">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" s="2">
+        <v>45565</v>
+      </c>
+      <c r="D46">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D47">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D48">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D49">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50" s="2">
+        <v>45322</v>
+      </c>
+      <c r="D50">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51" s="2">
+        <v>45351</v>
+      </c>
+      <c r="D51">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" s="2">
+        <v>45382</v>
+      </c>
+      <c r="D52">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53" s="2">
+        <v>45412</v>
+      </c>
+      <c r="D53">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54" s="2">
+        <v>45443</v>
+      </c>
+      <c r="D54">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55" s="2">
+        <v>45473</v>
+      </c>
+      <c r="D55">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D56">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57" s="2">
+        <v>45535</v>
+      </c>
+      <c r="D57">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>5</v>
+      </c>
+      <c r="C58" s="2">
+        <v>45565</v>
+      </c>
+      <c r="D58">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D59">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D60">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D61">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>6</v>
+      </c>
+      <c r="C62" s="2">
+        <v>45322</v>
+      </c>
+      <c r="D62">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>6</v>
+      </c>
+      <c r="C63" s="2">
+        <v>45351</v>
+      </c>
+      <c r="D63">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+      <c r="C64" s="2">
+        <v>45382</v>
+      </c>
+      <c r="D64">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>6</v>
+      </c>
+      <c r="C65" s="2">
+        <v>45412</v>
+      </c>
+      <c r="D65">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>6</v>
+      </c>
+      <c r="C66" s="2">
+        <v>45443</v>
+      </c>
+      <c r="D66">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>6</v>
+      </c>
+      <c r="C67" s="2">
+        <v>45473</v>
+      </c>
+      <c r="D67">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>6</v>
+      </c>
+      <c r="C68" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D68">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>6</v>
+      </c>
+      <c r="C69" s="2">
+        <v>45535</v>
+      </c>
+      <c r="D69">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>6</v>
+      </c>
+      <c r="C70" s="2">
+        <v>45565</v>
+      </c>
+      <c r="D70">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>6</v>
+      </c>
+      <c r="C71" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D71">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>6</v>
+      </c>
+      <c r="C72" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D72">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>6</v>
+      </c>
+      <c r="C73" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D73">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>7</v>
+      </c>
+      <c r="C74" s="2">
+        <v>45322</v>
+      </c>
+      <c r="D74">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>7</v>
+      </c>
+      <c r="C75" s="2">
+        <v>45351</v>
+      </c>
+      <c r="D75">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>7</v>
+      </c>
+      <c r="C76" s="2">
+        <v>45382</v>
+      </c>
+      <c r="D76">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>7</v>
+      </c>
+      <c r="C77" s="2">
+        <v>45412</v>
+      </c>
+      <c r="D77">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>7</v>
+      </c>
+      <c r="C78" s="2">
+        <v>45443</v>
+      </c>
+      <c r="D78">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>7</v>
+      </c>
+      <c r="C79" s="2">
+        <v>45473</v>
+      </c>
+      <c r="D79">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>7</v>
+      </c>
+      <c r="C80" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D80">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>7</v>
+      </c>
+      <c r="C81" s="2">
+        <v>45535</v>
+      </c>
+      <c r="D81">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>7</v>
+      </c>
+      <c r="C82" s="2">
+        <v>45565</v>
+      </c>
+      <c r="D82">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>7</v>
+      </c>
+      <c r="C83" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D83">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>7</v>
+      </c>
+      <c r="C84" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D84">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>7</v>
+      </c>
+      <c r="C85" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D85">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>8</v>
+      </c>
+      <c r="C86" s="2">
+        <v>45322</v>
+      </c>
+      <c r="D86">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>8</v>
+      </c>
+      <c r="C87" s="2">
+        <v>45351</v>
+      </c>
+      <c r="D87">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>8</v>
+      </c>
+      <c r="C88" s="2">
+        <v>45382</v>
+      </c>
+      <c r="D88">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>8</v>
+      </c>
+      <c r="C89" s="2">
+        <v>45412</v>
+      </c>
+      <c r="D89">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>8</v>
+      </c>
+      <c r="C90" s="2">
+        <v>45443</v>
+      </c>
+      <c r="D90">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>8</v>
+      </c>
+      <c r="C91" s="2">
+        <v>45473</v>
+      </c>
+      <c r="D91">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>8</v>
+      </c>
+      <c r="C92" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D92">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>8</v>
+      </c>
+      <c r="C93" s="2">
+        <v>45535</v>
+      </c>
+      <c r="D93">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>8</v>
+      </c>
+      <c r="C94" s="2">
+        <v>45565</v>
+      </c>
+      <c r="D94">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>8</v>
+      </c>
+      <c r="C95" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D95">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>8</v>
+      </c>
+      <c r="C96" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D96">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>8</v>
+      </c>
+      <c r="C97" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D97">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>9</v>
+      </c>
+      <c r="C98" s="2">
+        <v>45322</v>
+      </c>
+      <c r="D98">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>9</v>
+      </c>
+      <c r="C99" s="2">
+        <v>45351</v>
+      </c>
+      <c r="D99">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>9</v>
+      </c>
+      <c r="C100" s="2">
+        <v>45382</v>
+      </c>
+      <c r="D100">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>9</v>
+      </c>
+      <c r="C101" s="2">
+        <v>45412</v>
+      </c>
+      <c r="D101">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>9</v>
+      </c>
+      <c r="C102" s="2">
+        <v>45443</v>
+      </c>
+      <c r="D102">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>9</v>
+      </c>
+      <c r="C103" s="2">
+        <v>45473</v>
+      </c>
+      <c r="D103">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>9</v>
+      </c>
+      <c r="C104" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D104">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>9</v>
+      </c>
+      <c r="C105" s="2">
+        <v>45535</v>
+      </c>
+      <c r="D105">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>9</v>
+      </c>
+      <c r="C106" s="2">
+        <v>45565</v>
+      </c>
+      <c r="D106">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <v>9</v>
+      </c>
+      <c r="C107" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D107">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>9</v>
+      </c>
+      <c r="C108" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D108">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>9</v>
+      </c>
+      <c r="C109" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D109">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21E4E4C-FD36-4510-BF47-AA475E438994}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1266,13 +2814,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1283,10 +2831,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1297,10 +2845,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1311,10 +2859,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1325,10 +2873,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1339,10 +2887,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1353,10 +2901,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1367,10 +2915,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1381,10 +2929,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1395,10 +2943,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1409,10 +2957,10 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1423,10 +2971,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1437,10 +2985,10 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1451,10 +2999,10 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1465,10 +3013,10 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1479,10 +3027,10 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1493,10 +3041,10 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1507,10 +3055,10 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1521,10 +3069,10 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1535,10 +3083,10 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1549,10 +3097,10 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1563,10 +3111,10 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1577,10 +3125,10 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1591,10 +3139,10 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1605,10 +3153,10 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1619,10 +3167,10 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1633,10 +3181,10 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1647,10 +3195,10 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1661,10 +3209,10 @@
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1675,10 +3223,10 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1689,10 +3237,10 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1701,12 +3249,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE59B40-307D-455E-BAC3-8156BBBE35B6}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1733,7 +3281,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C2" s="2">
         <v>45292</v>
@@ -1747,7 +3295,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C3" s="2">
         <v>45323</v>
@@ -1761,7 +3309,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C4" s="2">
         <v>45352</v>
@@ -1775,7 +3323,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C5" s="2">
         <v>45383</v>
@@ -1789,7 +3337,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C6" s="2">
         <v>45413</v>
@@ -1803,7 +3351,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C7" s="2">
         <v>45444</v>
@@ -1817,7 +3365,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C8" s="2">
         <v>45474</v>
@@ -1831,7 +3379,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C9" s="2">
         <v>45505</v>
@@ -1845,7 +3393,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C10" s="2">
         <v>45536</v>
@@ -1859,7 +3407,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C11" s="2">
         <v>45566</v>
@@ -1873,7 +3421,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C12" s="2">
         <v>45597</v>
@@ -1887,7 +3435,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C13" s="2">
         <v>45627</v>
@@ -1901,7 +3449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD35900-BFB0-4F25-BD79-7AEF2D6AFBD4}">
   <dimension ref="A1:H91"/>
   <sheetViews>
@@ -1919,19 +3467,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>